<commit_message>
Restruturação das páginas: cad. usuario, usuarios cadastrados e menu adm
</commit_message>
<xml_diff>
--- a/Site institucional/Cronograma site.xlsx
+++ b/Site institucional/Cronograma site.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor\OneDrive\Área de Trabalho\BandTec\2º Semestre\Grupo_04-2ADSA\Site institucional\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DE643C-97FE-42B1-B08C-9B0657FD00AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DD043B-6C51-4F25-9CFF-200A616AA87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="41">
   <si>
     <t>Status</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Já está pronto</t>
   </si>
   <si>
-    <t>Mais ou menos</t>
-  </si>
-  <si>
     <t>Troca imagem, ajustar responsividade</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>Estrutura precisa ser atualizada para o novo menu</t>
   </si>
   <si>
     <t>Precisa fazer</t>
@@ -324,7 +318,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -620,7 +614,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,13 +630,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
+      <c r="E1" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -662,7 +656,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>0</v>
@@ -675,138 +669,138 @@
       <c r="C3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>24</v>
+      <c r="D3" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>21</v>
+      <c r="D5" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="E5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>21</v>
+      <c r="D6" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="E6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -814,19 +808,19 @@
         <v>12</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>18</v>
@@ -834,70 +828,70 @@
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="C10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="F10" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="12" t="s">
@@ -906,26 +900,26 @@
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="F13" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualização e construção de páginas
</commit_message>
<xml_diff>
--- a/Site institucional/Cronograma site.xlsx
+++ b/Site institucional/Cronograma site.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor\OneDrive\Área de Trabalho\BandTec\2º Semestre\Grupo_04-2ADSA\Site institucional\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93946925-5D12-4C70-9395-77C2A6B727DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9001CE60-23E9-41C4-AEA5-84055E2A27A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -611,7 +611,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -854,10 +854,10 @@
       <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="C11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="8" t="s">
@@ -881,7 +881,7 @@
       <c r="C12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="8" t="s">
@@ -905,7 +905,7 @@
       <c r="C13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="8" t="s">

</xml_diff>

<commit_message>
Atualização das páginas do site
</commit_message>
<xml_diff>
--- a/Site institucional/Cronograma site.xlsx
+++ b/Site institucional/Cronograma site.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor\OneDrive\Área de Trabalho\BandTec\2º Semestre\Grupo_04-2ADSA\Site institucional\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9001CE60-23E9-41C4-AEA5-84055E2A27A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D8D461-CD87-4629-8E63-32275711C265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
   <si>
     <t>Status</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>Falta a validação</t>
-  </si>
-  <si>
-    <t>Falta desenvolver</t>
   </si>
   <si>
     <t>X</t>
@@ -611,7 +608,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C12" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,13 +624,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -653,7 +650,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>0</v>
@@ -667,13 +664,13 @@
         <v>19</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="7" t="s">
@@ -682,7 +679,7 @@
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
@@ -691,7 +688,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>22</v>
@@ -706,7 +703,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -715,7 +712,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>22</v>
@@ -730,7 +727,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
@@ -739,7 +736,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>22</v>
@@ -754,7 +751,7 @@
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
@@ -763,13 +760,13 @@
         <v>19</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="7" t="s">
@@ -778,7 +775,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>14</v>
@@ -787,13 +784,13 @@
         <v>19</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="7" t="s">
@@ -805,19 +802,19 @@
         <v>12</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>18</v>
@@ -825,7 +822,7 @@
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>13</v>
@@ -834,13 +831,13 @@
         <v>19</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="7" t="s">
@@ -849,7 +846,7 @@
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>15</v>
@@ -858,22 +855,22 @@
         <v>19</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>16</v>
@@ -882,13 +879,13 @@
         <v>19</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="12" t="s">
@@ -897,26 +894,26 @@
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>24</v>
+      <c r="C13" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>